<commit_message>
updates to loading data and pipe
</commit_message>
<xml_diff>
--- a/data/raw/data_likert.xlsx
+++ b/data/raw/data_likert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian-Hussey/git/data-wrangling-and-visualization-course/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D8B80E-F627-454A-9872-765B10DA831E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23B969C-F7C7-D744-B860-69927D1EF6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{60EAE659-77DB-F447-8D9A-02BAB08D90F6}"/>
   </bookViews>
@@ -906,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C22849D-10DB-C845-8743-B51F7A0B47E3}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1026,91 +1026,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>44735</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>44735</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>44735</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>44735</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>9</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>44735</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1118,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047CA7D6-435A-C24D-B83D-4C663B5A826B}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="A10" sqref="A10:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1158,7 +1073,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1172,7 +1087,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1186,7 +1101,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -1200,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1214,80 +1129,10 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>44735</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>16</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>44735</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>17</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>44735</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>18</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>44735</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>19</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>44735</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>20</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>